<commit_message>
Finished the fixes, mod5 is a go
finished
</commit_message>
<xml_diff>
--- a/TimeLine-SDEV1031UpdatedForSchedule1.xlsx
+++ b/TimeLine-SDEV1031UpdatedForSchedule1.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Documents\SDEV1031afterch2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Documents\GitHub\SDEV1031\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861B3A52-99DE-499F-A7E4-7668100CCC63}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2705DC62-3E66-4B8F-8027-189338E7B520}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SDEV 1031" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -870,7 +865,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
@@ -889,6 +883,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -904,7 +899,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1187,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,7 +1328,9 @@
       <c r="G8" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="27"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="68"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="73">
@@ -1348,13 +1347,15 @@
         <v>43368</v>
       </c>
       <c r="E9" s="20"/>
-      <c r="F9" s="93">
+      <c r="F9" s="92">
         <v>43360</v>
       </c>
-      <c r="G9" s="94">
+      <c r="G9" s="93">
         <v>43369</v>
       </c>
-      <c r="K9" s="27"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="69"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="74">
@@ -1370,13 +1371,15 @@
         <v>43374</v>
       </c>
       <c r="E10" s="20"/>
-      <c r="F10" s="93">
+      <c r="F10" s="92">
         <v>43369</v>
       </c>
-      <c r="G10" s="95">
+      <c r="G10" s="94">
         <v>43404</v>
       </c>
-      <c r="K10" s="27"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="70"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="75">
@@ -1392,13 +1395,15 @@
         <v>43378</v>
       </c>
       <c r="E11" s="20"/>
-      <c r="F11" s="93">
+      <c r="F11" s="92">
         <v>43404</v>
       </c>
-      <c r="G11" s="94">
+      <c r="G11" s="93">
         <v>43410</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="70"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="76">
@@ -1414,11 +1419,15 @@
         <v>43384</v>
       </c>
       <c r="E12" s="20"/>
-      <c r="F12" s="103">
+      <c r="F12" s="95">
         <v>43412</v>
       </c>
-      <c r="G12" s="84"/>
-      <c r="K12" s="27"/>
+      <c r="G12" s="94">
+        <v>43431</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="70"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="77">
@@ -1434,9 +1443,13 @@
         <v>43396</v>
       </c>
       <c r="E13" s="20"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="84"/>
-      <c r="K13" s="27"/>
+      <c r="F13" s="95">
+        <v>43431</v>
+      </c>
+      <c r="G13" s="83"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="70"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="78">
@@ -1453,9 +1466,11 @@
         <v>43398</v>
       </c>
       <c r="E14" s="20"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="86"/>
-      <c r="K14" s="27"/>
+      <c r="F14" s="84"/>
+      <c r="G14" s="85"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="103"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="79"/>
@@ -1477,17 +1492,17 @@
       <c r="C16" s="67"/>
       <c r="D16" s="67"/>
       <c r="E16" s="66"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="91"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="90"/>
-      <c r="N16" s="90"/>
-      <c r="O16" s="90"/>
-      <c r="P16" s="90"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="91"/>
+      <c r="L16" s="89"/>
+      <c r="M16" s="89"/>
+      <c r="N16" s="89"/>
+      <c r="O16" s="89"/>
+      <c r="P16" s="89"/>
     </row>
     <row r="17" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
@@ -1791,7 +1806,7 @@
         <v>42066</v>
       </c>
       <c r="E31" s="20"/>
-      <c r="F31" s="87" t="s">
+      <c r="F31" s="86" t="s">
         <v>54</v>
       </c>
       <c r="G31" s="20"/>
@@ -1832,7 +1847,7 @@
         <v>42073</v>
       </c>
       <c r="E32" s="20"/>
-      <c r="F32" s="87" t="s">
+      <c r="F32" s="86" t="s">
         <v>55</v>
       </c>
       <c r="G32" s="20"/>
@@ -1865,7 +1880,7 @@
         <v>42080</v>
       </c>
       <c r="E33" s="5"/>
-      <c r="F33" s="88" t="s">
+      <c r="F33" s="87" t="s">
         <v>56</v>
       </c>
       <c r="G33" s="5"/>
@@ -1909,7 +1924,7 @@
         <v>42088</v>
       </c>
       <c r="E34" s="5"/>
-      <c r="F34" s="88" t="s">
+      <c r="F34" s="87" t="s">
         <v>57</v>
       </c>
       <c r="G34" s="5"/>
@@ -1950,7 +1965,7 @@
         <v>42094</v>
       </c>
       <c r="E35" s="5"/>
-      <c r="F35" s="88"/>
+      <c r="F35" s="87"/>
       <c r="G35" s="5"/>
       <c r="H35" s="57"/>
       <c r="I35" s="57"/>
@@ -1982,7 +1997,7 @@
         <v>43398</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="89"/>
+      <c r="F36" s="88"/>
       <c r="G36" s="1"/>
       <c r="H36" s="58">
         <v>42093</v>

</xml_diff>

<commit_message>
Im too tired to work
sorry
</commit_message>
<xml_diff>
--- a/TimeLine-SDEV1031UpdatedForSchedule1.xlsx
+++ b/TimeLine-SDEV1031UpdatedForSchedule1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Documents\SDEV1031afterch2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Documents\GitHub\SDEV1031\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB4B198-F340-4689-B628-38FA9E626B1B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A1A5B627-B84E-4930-B172-19AD6AC9B7BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -894,6 +894,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -909,7 +910,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1192,7 +1192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1214,12 +1214,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="101" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
@@ -1227,14 +1227,14 @@
       <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="97"/>
+      <c r="A2" s="98"/>
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="95">
+      <c r="C2" s="96">
         <v>43360</v>
       </c>
-      <c r="D2" s="95"/>
+      <c r="D2" s="96"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14" t="s">
         <v>50</v>
@@ -1244,14 +1244,14 @@
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="98"/>
       <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="96">
+      <c r="C3" s="97">
         <v>43398</v>
       </c>
-      <c r="D3" s="96"/>
+      <c r="D3" s="97"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -1259,7 +1259,7 @@
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
+      <c r="A4" s="98"/>
       <c r="B4" s="16" t="s">
         <v>3</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="97"/>
+      <c r="A5" s="98"/>
       <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
@@ -1289,7 +1289,7 @@
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="97"/>
+      <c r="A6" s="98"/>
       <c r="B6" s="17" t="s">
         <v>2</v>
       </c>
@@ -1304,10 +1304,10 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98"/>
-      <c r="B7" s="99"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
+      <c r="A7" s="99"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
       <c r="E7" s="14"/>
       <c r="F7" s="2" t="s">
         <v>49</v>
@@ -1479,7 +1479,7 @@
         <v>43398</v>
       </c>
       <c r="E14" s="20"/>
-      <c r="F14" s="102">
+      <c r="F14" s="95">
         <v>43445</v>
       </c>
       <c r="G14" s="83"/>

</xml_diff>